<commit_message>
First draft of C function.
</commit_message>
<xml_diff>
--- a/inst/extdata/GH-ZA-Allocation-sample-2019.xlsx
+++ b/inst/extdata/GH-ZA-Allocation-sample-2019.xlsx
@@ -1,21 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/IEATools/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/IEATools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F099DD-EC2D-764D-8002-EF80B965CD58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE457F92-7319-0946-BF2E-03D51BDCA308}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20460" yWindow="460" windowWidth="25520" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FU Allocations" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -399,21 +407,25 @@
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF104273"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF918700"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -779,9 +791,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O707"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A490" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O527" sqref="O527"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21814,7 +21826,7 @@
       <c r="M525" s="4"/>
       <c r="N525" s="7"/>
       <c r="O525" s="8">
-        <v>0.4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="526" spans="1:15" x14ac:dyDescent="0.2">
@@ -21850,9 +21862,7 @@
       </c>
       <c r="M526" s="4"/>
       <c r="N526" s="7"/>
-      <c r="O526" s="8">
-        <v>0.6</v>
-      </c>
+      <c r="O526" s="8"/>
     </row>
     <row r="527" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A527" t="s">

</xml_diff>

<commit_message>
Added new final row to sample allocation table.
</commit_message>
<xml_diff>
--- a/inst/extdata/GH-ZA-Allocation-sample-2019.xlsx
+++ b/inst/extdata/GH-ZA-Allocation-sample-2019.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/IEATools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE457F92-7319-0946-BF2E-03D51BDCA308}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4710D9C-DD61-CE40-8CE0-2A2BC82A053F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20460" yWindow="460" windowWidth="25520" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7439" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7449" uniqueCount="120">
   <si>
     <t>Country</t>
   </si>
@@ -789,11 +789,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O707"/>
+  <dimension ref="A1:O708"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A490" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O527" sqref="O527"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A644" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L708" sqref="L708"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -29061,6 +29061,41 @@
       <c r="N707" s="8"/>
       <c r="O707" s="8"/>
     </row>
+    <row r="708" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A708" t="s">
+        <v>53</v>
+      </c>
+      <c r="B708" t="s">
+        <v>16</v>
+      </c>
+      <c r="C708" t="s">
+        <v>17</v>
+      </c>
+      <c r="D708" t="s">
+        <v>18</v>
+      </c>
+      <c r="E708" t="s">
+        <v>31</v>
+      </c>
+      <c r="F708" t="s">
+        <v>47</v>
+      </c>
+      <c r="G708" t="s">
+        <v>21</v>
+      </c>
+      <c r="H708" t="s">
+        <v>29</v>
+      </c>
+      <c r="K708" t="s">
+        <v>78</v>
+      </c>
+      <c r="L708" t="s">
+        <v>97</v>
+      </c>
+      <c r="M708" s="4"/>
+      <c r="N708" s="8"/>
+      <c r="O708" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Wood stoves --> Wood cookstoves
</commit_message>
<xml_diff>
--- a/inst/extdata/GH-ZA-Allocation-sample-2019.xlsx
+++ b/inst/extdata/GH-ZA-Allocation-sample-2019.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/IEATools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D66021-682A-7942-B350-A8E4D6926174}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18EC6C0-E92F-B945-992F-A0C405B3B8F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="31380" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,6 @@
     <sheet name="FU Allocations" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -828,8 +820,8 @@
   <dimension ref="A1:O754"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I165" sqref="I165"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I140" sqref="I140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4858,7 +4850,7 @@
         <v>41</v>
       </c>
       <c r="I99" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="J99" t="s">
         <v>92</v>
@@ -5912,7 +5904,7 @@
         <v>41</v>
       </c>
       <c r="I125" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="J125" t="s">
         <v>92</v>
@@ -6519,7 +6511,7 @@
         <v>41</v>
       </c>
       <c r="I140" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="J140" t="s">
         <v>92</v>

</xml_diff>